<commit_message>
Progresos Dia Martes 09 06 2020
</commit_message>
<xml_diff>
--- a/Progresos/Hitos importantes.xlsx
+++ b/Progresos/Hitos importantes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Objetivo del documento: </t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entendí cómo se ampliaban las opciones en la cadena. Si no encuentro un strike específico, ponerle ALL para que me muestre todo. Ahí ya me va a salir todo. </t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,10 +412,21 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>43989</v>
+        <v>44018</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44049</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicion de nuevos hitos
</commit_message>
<xml_diff>
--- a/Progresos/Hitos importantes.xlsx
+++ b/Progresos/Hitos importantes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Objetivo del documento: </t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve">Entendí cómo se ampliaban las opciones en la cadena. Si no encuentro un strike específico, ponerle ALL para que me muestre todo. Ahí ya me va a salir todo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leí sobre Transferwise. Genial está. Probablemente de ahí podré transferir fondos y recibir mis ganancias de TradeStation. Y de Zulutrade en Skrill. Y después, todo a Payoneer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vi que no me ejecutó cierta orden de BPCS de TSLA. Mary me dijo que podría ser por mi nivel 1 en TS. Tengo que ver para aumentar sus fondos. </t>
   </si>
 </sst>
 </file>
@@ -364,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -372,14 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="174.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -429,6 +439,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>44080</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>44110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Primer commit anho actualizacion 2021 PEDEM
</commit_message>
<xml_diff>
--- a/Progresos/Hitos importantes.xlsx
+++ b/Progresos/Hitos importantes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
   <si>
     <t xml:space="preserve">Objetivo del documento: </t>
   </si>
@@ -424,6 +424,24 @@
   </si>
   <si>
     <t xml:space="preserve">También voy a tratar de practicar algo de EasyLanguage. Creo que no es muy complicado. Un poquito por lo menos. En un año, ya podría crear un bot experto. </t>
+  </si>
+  <si>
+    <t>14/09/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aprendí a usar ordenes OSO. Me ahorra tiempo. </t>
+  </si>
+  <si>
+    <t>Esta semana volví completamente a demo. Quiero terminar mis 20 operaciones para tener una estrategia. Ya sea de scalping o El normal. Mejor abrir operacione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s en la hora de la sesión americana. O sino, Desde las 09:00 a las 16:00hs como dijo un compañero. Legalmente empieza a haber más volatilidad a partir de las </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoy levanté mi primer vídeo en mi Canal de Youtube exclusiva para alzar el entrenamiento: KAIZEN 4 LIVE. Pienso que podría hacer una comparación con el que suele levantar JAVA Trading. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayer aprendí algo muy importante que dijo Oliver Velez. Es mejor perder futuras ganancias, que perder capital. </t>
   </si>
 </sst>
 </file>
@@ -497,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,6 +547,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -835,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView topLeftCell="B64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="B70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,8 +1541,12 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
+      <c r="B86" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
@@ -1530,8 +1555,12 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
+      <c r="B88" s="14">
+        <v>44053</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
@@ -1540,8 +1569,12 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
+      <c r="B90" s="14">
+        <v>43872</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
@@ -1878,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G128"/>
   <sheetViews>
-    <sheetView topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView topLeftCell="D50" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,7 +1965,7 @@
       <c r="B8" s="11">
         <v>44018</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="16">
         <v>1</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -1956,7 +1989,7 @@
       <c r="B9" s="11">
         <v>44019</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="10" t="s">
         <v>68</v>
       </c>
@@ -1975,7 +2008,7 @@
       <c r="B10" s="11">
         <v>44020</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="10" t="s">
         <v>68</v>
       </c>
@@ -1994,7 +2027,7 @@
       <c r="B11" s="11">
         <v>44021</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="10" t="s">
         <v>68</v>
       </c>
@@ -2013,7 +2046,7 @@
       <c r="B12" s="11">
         <v>44022</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="10" t="s">
         <v>68</v>
       </c>
@@ -2032,7 +2065,7 @@
       <c r="B13" s="11">
         <v>44025</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="16">
         <v>2</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -2053,7 +2086,7 @@
       <c r="B14" s="11">
         <v>44026</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="10" t="s">
         <v>68</v>
       </c>
@@ -2072,7 +2105,7 @@
       <c r="B15" s="11">
         <v>44027</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="10" t="s">
         <v>68</v>
       </c>
@@ -2091,7 +2124,7 @@
       <c r="B16" s="11">
         <v>44028</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="10" t="s">
         <v>68</v>
       </c>
@@ -2110,7 +2143,7 @@
       <c r="B17" s="11">
         <v>44029</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="10" t="s">
         <v>68</v>
       </c>
@@ -2132,7 +2165,7 @@
       <c r="B18" s="11">
         <v>44032</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="16">
         <v>3</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -2153,7 +2186,7 @@
       <c r="B19" s="11">
         <v>44033</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="10" t="s">
         <v>68</v>
       </c>
@@ -2175,7 +2208,7 @@
       <c r="B20" s="11">
         <v>44034</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="10" t="s">
         <v>68</v>
       </c>
@@ -2197,7 +2230,7 @@
       <c r="B21" s="11">
         <v>44035</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="10" t="s">
         <v>68</v>
       </c>
@@ -2216,7 +2249,7 @@
       <c r="B22" s="11">
         <v>44036</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="10" t="s">
         <v>68</v>
       </c>
@@ -2235,7 +2268,7 @@
       <c r="B23" s="11">
         <v>44039</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="16">
         <v>4</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -2256,7 +2289,7 @@
       <c r="B24" s="11">
         <v>44040</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="10" t="s">
         <v>68</v>
       </c>
@@ -2275,7 +2308,7 @@
       <c r="B25" s="11">
         <v>44041</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="10" t="s">
         <v>68</v>
       </c>
@@ -2294,7 +2327,7 @@
       <c r="B26" s="11">
         <v>44042</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="10" t="s">
         <v>68</v>
       </c>
@@ -2313,7 +2346,7 @@
       <c r="B27" s="11">
         <v>44043</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="10" t="s">
         <v>68</v>
       </c>
@@ -2332,7 +2365,7 @@
       <c r="B28" s="11">
         <v>44046</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="16">
         <v>5</v>
       </c>
       <c r="D28" s="10" t="s">
@@ -2356,7 +2389,7 @@
       <c r="B29" s="11">
         <v>44047</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="10" t="s">
         <v>68</v>
       </c>
@@ -2375,7 +2408,7 @@
       <c r="B30" s="11">
         <v>44048</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="10" t="s">
         <v>68</v>
       </c>
@@ -2394,7 +2427,7 @@
       <c r="B31" s="11">
         <v>44049</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="10" t="s">
         <v>68</v>
       </c>
@@ -2413,7 +2446,7 @@
       <c r="B32" s="11">
         <v>44050</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="10" t="s">
         <v>68</v>
       </c>
@@ -2432,7 +2465,7 @@
       <c r="B33" s="11">
         <v>44053</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="16">
         <v>6</v>
       </c>
       <c r="D33" s="10" t="s">
@@ -2453,7 +2486,7 @@
       <c r="B34" s="11">
         <v>44054</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="10" t="s">
         <v>68</v>
       </c>
@@ -2475,7 +2508,7 @@
       <c r="B35" s="11">
         <v>44055</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="10" t="s">
         <v>68</v>
       </c>
@@ -2497,7 +2530,7 @@
       <c r="B36" s="11">
         <v>44056</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="10" t="s">
         <v>68</v>
       </c>
@@ -2519,7 +2552,7 @@
       <c r="B37" s="11">
         <v>44057</v>
       </c>
-      <c r="C37" s="15"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="10" t="s">
         <v>68</v>
       </c>
@@ -2541,7 +2574,7 @@
       <c r="B38" s="11">
         <v>44060</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="16">
         <v>7</v>
       </c>
       <c r="D38" s="10" t="s">
@@ -2565,7 +2598,7 @@
       <c r="B39" s="11">
         <v>44061</v>
       </c>
-      <c r="C39" s="15"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="10" t="s">
         <v>73</v>
       </c>
@@ -2587,7 +2620,7 @@
       <c r="B40" s="11">
         <v>44062</v>
       </c>
-      <c r="C40" s="15"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="10" t="s">
         <v>73</v>
       </c>
@@ -2609,7 +2642,7 @@
       <c r="B41" s="11">
         <v>44063</v>
       </c>
-      <c r="C41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="10" t="s">
         <v>73</v>
       </c>
@@ -2631,7 +2664,7 @@
       <c r="B42" s="13">
         <v>44064</v>
       </c>
-      <c r="C42" s="15"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="10" t="s">
         <v>73</v>
       </c>
@@ -2653,7 +2686,7 @@
       <c r="B43" s="11">
         <v>44067</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="16">
         <v>8</v>
       </c>
       <c r="D43" s="10" t="s">
@@ -2677,7 +2710,7 @@
       <c r="B44" s="11">
         <v>44068</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="10" t="s">
         <v>73</v>
       </c>
@@ -2699,7 +2732,7 @@
       <c r="B45" s="11">
         <v>44069</v>
       </c>
-      <c r="C45" s="15"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="10" t="s">
         <v>73</v>
       </c>
@@ -2721,7 +2754,7 @@
       <c r="B46" s="11">
         <v>44070</v>
       </c>
-      <c r="C46" s="15"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="10" t="s">
         <v>73</v>
       </c>
@@ -2743,7 +2776,7 @@
       <c r="B47" s="11">
         <v>44071</v>
       </c>
-      <c r="C47" s="15"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="10" t="s">
         <v>73</v>
       </c>
@@ -2765,7 +2798,7 @@
       <c r="B48" s="11">
         <v>44074</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="16">
         <v>9</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -2778,219 +2811,238 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>42</v>
       </c>
       <c r="B49" s="11">
         <v>44075</v>
       </c>
-      <c r="C49" s="15"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>43</v>
       </c>
       <c r="B50" s="11">
         <v>44076</v>
       </c>
-      <c r="C50" s="15"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>44</v>
       </c>
       <c r="B51" s="11">
         <v>44077</v>
       </c>
-      <c r="C51" s="15"/>
+      <c r="C51" s="16"/>
       <c r="D51" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>45</v>
       </c>
       <c r="B52" s="11">
         <v>44078</v>
       </c>
-      <c r="C52" s="15"/>
+      <c r="C52" s="16"/>
       <c r="D52" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>46</v>
       </c>
       <c r="B53" s="11">
         <v>44081</v>
       </c>
-      <c r="C53" s="15">
+      <c r="C53" s="16">
         <v>10</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>47</v>
       </c>
       <c r="B54" s="11">
         <v>44082</v>
       </c>
-      <c r="C54" s="15"/>
+      <c r="C54" s="16"/>
       <c r="D54" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>48</v>
       </c>
       <c r="B55" s="11">
         <v>44083</v>
       </c>
-      <c r="C55" s="15"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>49</v>
       </c>
       <c r="B56" s="11">
         <v>44084</v>
       </c>
-      <c r="C56" s="15"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E56" s="10"/>
-    </row>
-    <row r="57" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>50</v>
       </c>
       <c r="B57" s="11">
         <v>44085</v>
       </c>
-      <c r="C57" s="15"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>51</v>
       </c>
       <c r="B58" s="11">
         <v>44088</v>
       </c>
-      <c r="C58" s="15">
+      <c r="C58" s="16">
         <v>11</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E58" s="10"/>
-    </row>
-    <row r="59" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>52</v>
       </c>
       <c r="B59" s="11">
         <v>44089</v>
       </c>
-      <c r="C59" s="15"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E59" s="10"/>
-    </row>
-    <row r="60" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>53</v>
       </c>
       <c r="B60" s="11">
         <v>44090</v>
       </c>
-      <c r="C60" s="15"/>
+      <c r="C60" s="16"/>
       <c r="D60" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E60" s="10"/>
-    </row>
-    <row r="61" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>54</v>
       </c>
       <c r="B61" s="11">
         <v>44091</v>
       </c>
-      <c r="C61" s="15"/>
+      <c r="C61" s="16"/>
       <c r="D61" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E61" s="10"/>
-    </row>
-    <row r="62" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>55</v>
       </c>
       <c r="B62" s="11">
         <v>44092</v>
       </c>
-      <c r="C62" s="15"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E62" s="10"/>
-    </row>
-    <row r="63" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>56</v>
       </c>
       <c r="B63" s="11">
         <v>44095</v>
       </c>
-      <c r="C63" s="15">
+      <c r="C63" s="16">
         <v>12</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E63" s="10"/>
-    </row>
-    <row r="64" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>57</v>
       </c>
       <c r="B64" s="11">
         <v>44096</v>
       </c>
-      <c r="C64" s="15"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E64" s="10"/>
+      <c r="F64"/>
+      <c r="G64" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
@@ -2999,11 +3051,14 @@
       <c r="B65" s="11">
         <v>44097</v>
       </c>
-      <c r="C65" s="15"/>
+      <c r="C65" s="16"/>
       <c r="D65" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E65" s="10"/>
+      <c r="G65" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
@@ -3012,11 +3067,14 @@
       <c r="B66" s="11">
         <v>44098</v>
       </c>
-      <c r="C66" s="15"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="10" t="s">
         <v>73</v>
       </c>
       <c r="E66" s="10"/>
+      <c r="G66" s="15">
+        <v>0.39583333333333331</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
@@ -3025,7 +3083,7 @@
       <c r="B67" s="13">
         <v>44099</v>
       </c>
-      <c r="C67" s="15"/>
+      <c r="C67" s="16"/>
       <c r="D67" s="10" t="s">
         <v>73</v>
       </c>
@@ -3038,7 +3096,7 @@
       <c r="B68" s="11">
         <v>44102</v>
       </c>
-      <c r="C68" s="15">
+      <c r="C68" s="16">
         <v>13</v>
       </c>
       <c r="D68" s="10" t="s">
@@ -3056,7 +3114,7 @@
       <c r="B69" s="11">
         <v>44103</v>
       </c>
-      <c r="C69" s="15"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="10" t="s">
         <v>74</v>
       </c>
@@ -3069,7 +3127,7 @@
       <c r="B70" s="11">
         <v>44104</v>
       </c>
-      <c r="C70" s="15"/>
+      <c r="C70" s="16"/>
       <c r="D70" s="10" t="s">
         <v>74</v>
       </c>
@@ -3082,7 +3140,7 @@
       <c r="B71" s="11">
         <v>44105</v>
       </c>
-      <c r="C71" s="15"/>
+      <c r="C71" s="16"/>
       <c r="D71" s="10" t="s">
         <v>74</v>
       </c>
@@ -3095,7 +3153,7 @@
       <c r="B72" s="11">
         <v>44106</v>
       </c>
-      <c r="C72" s="15"/>
+      <c r="C72" s="16"/>
       <c r="D72" s="10" t="s">
         <v>74</v>
       </c>
@@ -3108,7 +3166,7 @@
       <c r="B73" s="11">
         <v>44109</v>
       </c>
-      <c r="C73" s="15">
+      <c r="C73" s="16">
         <v>14</v>
       </c>
       <c r="D73" s="10" t="s">
@@ -3123,7 +3181,7 @@
       <c r="B74" s="11">
         <v>44110</v>
       </c>
-      <c r="C74" s="15"/>
+      <c r="C74" s="16"/>
       <c r="D74" s="10" t="s">
         <v>74</v>
       </c>
@@ -3136,7 +3194,7 @@
       <c r="B75" s="11">
         <v>44111</v>
       </c>
-      <c r="C75" s="15"/>
+      <c r="C75" s="16"/>
       <c r="D75" s="10" t="s">
         <v>74</v>
       </c>
@@ -3149,7 +3207,7 @@
       <c r="B76" s="11">
         <v>44112</v>
       </c>
-      <c r="C76" s="15"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="10" t="s">
         <v>74</v>
       </c>
@@ -3162,7 +3220,7 @@
       <c r="B77" s="11">
         <v>44113</v>
       </c>
-      <c r="C77" s="15"/>
+      <c r="C77" s="16"/>
       <c r="D77" s="10" t="s">
         <v>74</v>
       </c>
@@ -3175,7 +3233,7 @@
       <c r="B78" s="11">
         <v>44116</v>
       </c>
-      <c r="C78" s="15">
+      <c r="C78" s="16">
         <v>15</v>
       </c>
       <c r="D78" s="10" t="s">
@@ -3190,7 +3248,7 @@
       <c r="B79" s="11">
         <v>44117</v>
       </c>
-      <c r="C79" s="15"/>
+      <c r="C79" s="16"/>
       <c r="D79" s="10" t="s">
         <v>74</v>
       </c>
@@ -3203,7 +3261,7 @@
       <c r="B80" s="11">
         <v>44118</v>
       </c>
-      <c r="C80" s="15"/>
+      <c r="C80" s="16"/>
       <c r="D80" s="10" t="s">
         <v>74</v>
       </c>
@@ -3216,7 +3274,7 @@
       <c r="B81" s="11">
         <v>44119</v>
       </c>
-      <c r="C81" s="15"/>
+      <c r="C81" s="16"/>
       <c r="D81" s="10" t="s">
         <v>74</v>
       </c>
@@ -3229,7 +3287,7 @@
       <c r="B82" s="11">
         <v>44120</v>
       </c>
-      <c r="C82" s="15"/>
+      <c r="C82" s="16"/>
       <c r="D82" s="10" t="s">
         <v>74</v>
       </c>
@@ -3242,7 +3300,7 @@
       <c r="B83" s="11">
         <v>44123</v>
       </c>
-      <c r="C83" s="15">
+      <c r="C83" s="16">
         <v>16</v>
       </c>
       <c r="D83" s="10" t="s">
@@ -3257,7 +3315,7 @@
       <c r="B84" s="11">
         <v>44124</v>
       </c>
-      <c r="C84" s="15"/>
+      <c r="C84" s="16"/>
       <c r="D84" s="10" t="s">
         <v>74</v>
       </c>
@@ -3270,7 +3328,7 @@
       <c r="B85" s="11">
         <v>44125</v>
       </c>
-      <c r="C85" s="15"/>
+      <c r="C85" s="16"/>
       <c r="D85" s="10" t="s">
         <v>74</v>
       </c>
@@ -3283,7 +3341,7 @@
       <c r="B86" s="11">
         <v>44126</v>
       </c>
-      <c r="C86" s="15"/>
+      <c r="C86" s="16"/>
       <c r="D86" s="10" t="s">
         <v>74</v>
       </c>
@@ -3296,7 +3354,7 @@
       <c r="B87" s="11">
         <v>44127</v>
       </c>
-      <c r="C87" s="15"/>
+      <c r="C87" s="16"/>
       <c r="D87" s="10" t="s">
         <v>74</v>
       </c>
@@ -3309,7 +3367,7 @@
       <c r="B88" s="11">
         <v>44130</v>
       </c>
-      <c r="C88" s="15">
+      <c r="C88" s="16">
         <v>17</v>
       </c>
       <c r="D88" s="10" t="s">
@@ -3324,7 +3382,7 @@
       <c r="B89" s="11">
         <v>44131</v>
       </c>
-      <c r="C89" s="15"/>
+      <c r="C89" s="16"/>
       <c r="D89" s="10" t="s">
         <v>74</v>
       </c>
@@ -3337,7 +3395,7 @@
       <c r="B90" s="11">
         <v>44132</v>
       </c>
-      <c r="C90" s="15"/>
+      <c r="C90" s="16"/>
       <c r="D90" s="10" t="s">
         <v>74</v>
       </c>
@@ -3350,7 +3408,7 @@
       <c r="B91" s="11">
         <v>44133</v>
       </c>
-      <c r="C91" s="15"/>
+      <c r="C91" s="16"/>
       <c r="D91" s="10" t="s">
         <v>74</v>
       </c>
@@ -3363,7 +3421,7 @@
       <c r="B92" s="11">
         <v>44134</v>
       </c>
-      <c r="C92" s="15"/>
+      <c r="C92" s="16"/>
       <c r="D92" s="10" t="s">
         <v>74</v>
       </c>
@@ -3376,7 +3434,7 @@
       <c r="B93" s="11">
         <v>44137</v>
       </c>
-      <c r="C93" s="15">
+      <c r="C93" s="16">
         <v>18</v>
       </c>
       <c r="D93" s="10" t="s">
@@ -3391,7 +3449,7 @@
       <c r="B94" s="11">
         <v>44138</v>
       </c>
-      <c r="C94" s="15"/>
+      <c r="C94" s="16"/>
       <c r="D94" s="10" t="s">
         <v>74</v>
       </c>
@@ -3404,7 +3462,7 @@
       <c r="B95" s="11">
         <v>44139</v>
       </c>
-      <c r="C95" s="15"/>
+      <c r="C95" s="16"/>
       <c r="D95" s="10" t="s">
         <v>74</v>
       </c>
@@ -3417,7 +3475,7 @@
       <c r="B96" s="11">
         <v>44140</v>
       </c>
-      <c r="C96" s="15"/>
+      <c r="C96" s="16"/>
       <c r="D96" s="10" t="s">
         <v>74</v>
       </c>
@@ -3430,7 +3488,7 @@
       <c r="B97" s="11">
         <v>44141</v>
       </c>
-      <c r="C97" s="15"/>
+      <c r="C97" s="16"/>
       <c r="D97" s="10" t="s">
         <v>74</v>
       </c>
@@ -3443,7 +3501,7 @@
       <c r="B98" s="11">
         <v>44144</v>
       </c>
-      <c r="C98" s="15">
+      <c r="C98" s="16">
         <v>19</v>
       </c>
       <c r="D98" s="10" t="s">
@@ -3458,7 +3516,7 @@
       <c r="B99" s="11">
         <v>44145</v>
       </c>
-      <c r="C99" s="15"/>
+      <c r="C99" s="16"/>
       <c r="D99" s="10" t="s">
         <v>74</v>
       </c>
@@ -3471,7 +3529,7 @@
       <c r="B100" s="11">
         <v>44146</v>
       </c>
-      <c r="C100" s="15"/>
+      <c r="C100" s="16"/>
       <c r="D100" s="10" t="s">
         <v>74</v>
       </c>
@@ -3484,7 +3542,7 @@
       <c r="B101" s="11">
         <v>44147</v>
       </c>
-      <c r="C101" s="15"/>
+      <c r="C101" s="16"/>
       <c r="D101" s="10" t="s">
         <v>74</v>
       </c>
@@ -3497,7 +3555,7 @@
       <c r="B102" s="11">
         <v>44148</v>
       </c>
-      <c r="C102" s="15"/>
+      <c r="C102" s="16"/>
       <c r="D102" s="10" t="s">
         <v>74</v>
       </c>
@@ -3510,7 +3568,7 @@
       <c r="B103" s="11">
         <v>44151</v>
       </c>
-      <c r="C103" s="15">
+      <c r="C103" s="16">
         <v>20</v>
       </c>
       <c r="D103" s="10" t="s">
@@ -3525,7 +3583,7 @@
       <c r="B104" s="11">
         <v>44152</v>
       </c>
-      <c r="C104" s="15"/>
+      <c r="C104" s="16"/>
       <c r="D104" s="10" t="s">
         <v>74</v>
       </c>
@@ -3538,7 +3596,7 @@
       <c r="B105" s="11">
         <v>44153</v>
       </c>
-      <c r="C105" s="15"/>
+      <c r="C105" s="16"/>
       <c r="D105" s="10" t="s">
         <v>74</v>
       </c>
@@ -3551,7 +3609,7 @@
       <c r="B106" s="11">
         <v>44154</v>
       </c>
-      <c r="C106" s="15"/>
+      <c r="C106" s="16"/>
       <c r="D106" s="10" t="s">
         <v>74</v>
       </c>
@@ -3564,7 +3622,7 @@
       <c r="B107" s="11">
         <v>44155</v>
       </c>
-      <c r="C107" s="15"/>
+      <c r="C107" s="16"/>
       <c r="D107" s="10" t="s">
         <v>74</v>
       </c>
@@ -3577,7 +3635,7 @@
       <c r="B108" s="11">
         <v>44158</v>
       </c>
-      <c r="C108" s="15">
+      <c r="C108" s="16">
         <v>21</v>
       </c>
       <c r="D108" s="10" t="s">
@@ -3592,7 +3650,7 @@
       <c r="B109" s="11">
         <v>44159</v>
       </c>
-      <c r="C109" s="15"/>
+      <c r="C109" s="16"/>
       <c r="D109" s="10" t="s">
         <v>74</v>
       </c>
@@ -3605,7 +3663,7 @@
       <c r="B110" s="11">
         <v>44160</v>
       </c>
-      <c r="C110" s="15"/>
+      <c r="C110" s="16"/>
       <c r="D110" s="10" t="s">
         <v>74</v>
       </c>
@@ -3618,7 +3676,7 @@
       <c r="B111" s="11">
         <v>44161</v>
       </c>
-      <c r="C111" s="15"/>
+      <c r="C111" s="16"/>
       <c r="D111" s="10" t="s">
         <v>74</v>
       </c>
@@ -3631,7 +3689,7 @@
       <c r="B112" s="11">
         <v>44162</v>
       </c>
-      <c r="C112" s="15"/>
+      <c r="C112" s="16"/>
       <c r="D112" s="10" t="s">
         <v>74</v>
       </c>
@@ -3644,7 +3702,7 @@
       <c r="B113" s="11">
         <v>44165</v>
       </c>
-      <c r="C113" s="15">
+      <c r="C113" s="16">
         <v>22</v>
       </c>
       <c r="D113" s="10" t="s">
@@ -3659,7 +3717,7 @@
       <c r="B114" s="11">
         <v>44166</v>
       </c>
-      <c r="C114" s="15"/>
+      <c r="C114" s="16"/>
       <c r="D114" s="10" t="s">
         <v>74</v>
       </c>
@@ -3672,7 +3730,7 @@
       <c r="B115" s="11">
         <v>44167</v>
       </c>
-      <c r="C115" s="15"/>
+      <c r="C115" s="16"/>
       <c r="D115" s="10" t="s">
         <v>74</v>
       </c>
@@ -3685,7 +3743,7 @@
       <c r="B116" s="11">
         <v>44168</v>
       </c>
-      <c r="C116" s="15"/>
+      <c r="C116" s="16"/>
       <c r="D116" s="10" t="s">
         <v>74</v>
       </c>
@@ -3698,7 +3756,7 @@
       <c r="B117" s="11">
         <v>44169</v>
       </c>
-      <c r="C117" s="15"/>
+      <c r="C117" s="16"/>
       <c r="D117" s="10" t="s">
         <v>74</v>
       </c>
@@ -3711,7 +3769,7 @@
       <c r="B118" s="11">
         <v>44172</v>
       </c>
-      <c r="C118" s="15">
+      <c r="C118" s="16">
         <v>23</v>
       </c>
       <c r="D118" s="10" t="s">
@@ -3726,7 +3784,7 @@
       <c r="B119" s="11">
         <v>44173</v>
       </c>
-      <c r="C119" s="15"/>
+      <c r="C119" s="16"/>
       <c r="D119" s="10" t="s">
         <v>74</v>
       </c>
@@ -3739,7 +3797,7 @@
       <c r="B120" s="11">
         <v>44174</v>
       </c>
-      <c r="C120" s="15"/>
+      <c r="C120" s="16"/>
       <c r="D120" s="10" t="s">
         <v>74</v>
       </c>
@@ -3752,7 +3810,7 @@
       <c r="B121" s="11">
         <v>44175</v>
       </c>
-      <c r="C121" s="15"/>
+      <c r="C121" s="16"/>
       <c r="D121" s="10" t="s">
         <v>74</v>
       </c>
@@ -3765,7 +3823,7 @@
       <c r="B122" s="11">
         <v>44176</v>
       </c>
-      <c r="C122" s="15"/>
+      <c r="C122" s="16"/>
       <c r="D122" s="10" t="s">
         <v>74</v>
       </c>
@@ -3778,7 +3836,7 @@
       <c r="B123" s="11">
         <v>44179</v>
       </c>
-      <c r="C123" s="15">
+      <c r="C123" s="16">
         <v>24</v>
       </c>
       <c r="D123" s="10" t="s">
@@ -3793,7 +3851,7 @@
       <c r="B124" s="11">
         <v>44180</v>
       </c>
-      <c r="C124" s="15"/>
+      <c r="C124" s="16"/>
       <c r="D124" s="10" t="s">
         <v>74</v>
       </c>
@@ -3806,7 +3864,7 @@
       <c r="B125" s="11">
         <v>44181</v>
       </c>
-      <c r="C125" s="15"/>
+      <c r="C125" s="16"/>
       <c r="D125" s="10" t="s">
         <v>74</v>
       </c>
@@ -3819,7 +3877,7 @@
       <c r="B126" s="11">
         <v>44182</v>
       </c>
-      <c r="C126" s="15"/>
+      <c r="C126" s="16"/>
       <c r="D126" s="10" t="s">
         <v>74</v>
       </c>
@@ -3832,7 +3890,7 @@
       <c r="B127" s="11">
         <v>44183</v>
       </c>
-      <c r="C127" s="15"/>
+      <c r="C127" s="16"/>
       <c r="D127" s="10" t="s">
         <v>74</v>
       </c>
@@ -3877,7 +3935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>